<commit_message>
update model & more
</commit_message>
<xml_diff>
--- a/T3-Reports/T3_query_091420.xlsx
+++ b/T3-Reports/T3_query_091420.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeenatbaig/Documents/GitHub/order-book-project-team-3/T3-Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louie/NetBeansProjects/mthree_projects/order-book-project-team-3/T3-Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744AA0F-9F8C-C249-887F-E13F31BA9C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2627D66C-3BF5-BF4B-B0FB-4DD7ECEE25C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{DDA712E8-6EDA-4238-8DA3-86257BCBAB72}"/>
+    <workbookView xWindow="-23600" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{DDA712E8-6EDA-4238-8DA3-86257BCBAB72}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -24,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>PROJECT NAME/TEAM:</t>
   </si>
@@ -163,6 +155,21 @@
   </si>
   <si>
     <t xml:space="preserve">Zeenat </t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>should the user be able to place a order from the client side or orders are only to come from external source e.g manually inserting into the database ?</t>
   </si>
 </sst>
 </file>
@@ -890,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E078EC2-A1C0-4820-B2BA-09111DDDDDA4}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1011,7 +1018,9 @@
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1047,9 @@
       <c r="B10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1064,9 @@
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
+      <c r="J10" s="17">
+        <v>44088</v>
+      </c>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="84" x14ac:dyDescent="0.2">
@@ -1063,7 +1076,9 @@
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1078,7 +1093,9 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="17">
+        <v>44088</v>
+      </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="140" x14ac:dyDescent="0.2">
@@ -1088,7 +1105,9 @@
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1103,7 +1122,9 @@
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
+      <c r="J12" s="17">
+        <v>44088</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="84" x14ac:dyDescent="0.2">
@@ -1113,7 +1134,9 @@
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1128,7 +1151,9 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="J13" s="17">
+        <v>44088</v>
+      </c>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="70" x14ac:dyDescent="0.2">
@@ -1138,7 +1163,9 @@
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1151,7 +1178,9 @@
       <c r="G14" s="17"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17">
+        <v>44088</v>
+      </c>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="112" x14ac:dyDescent="0.2">
@@ -1161,7 +1190,9 @@
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1179,14 +1210,26 @@
       <c r="J15" s="17"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="154" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="17"/>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="17">
+        <v>44088</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
       <c r="J16" s="17"/>
@@ -1244,23 +1287,42 @@
       <c r="J20" s="17"/>
       <c r="K20" s="3"/>
     </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C16" xr:uid="{EC346FC3-6BE5-3B43-8D7C-3C0E19504DE1}">
+      <formula1>A26:A28</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{663FF8DE-C690-453E-BFD4-F766CB0281F7}">
           <x14:formula1>
             <xm:f>[QueryLog_FERS_R1_TMPL.xlsx]Setup!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>I9:I20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87F21C1B-9AA9-4486-B46C-C01EA64EEF40}">
-          <x14:formula1>
-            <xm:f>[QueryLog_FERS_R1_TMPL.xlsx]Setup!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9:C20 H9:H20</xm:sqref>
+          <xm:sqref>H9:I20 C17:C20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>